<commit_message>
0.1.1: translated common roles
translated 273 words
</commit_message>
<xml_diff>
--- a/tradept/Excel/Localization/english/R人物列表_Roles_Common_hotfix.xlsx
+++ b/tradept/Excel/Localization/english/R人物列表_Roles_Common_hotfix.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xargs01\Downloads\trasl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\tradept\Excel\Localization\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4F4B87-C92A-42EB-BEEE-BA9DC6FBFF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2952049F-AF6C-4634-896A-22A27FAD1549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="1290" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="319">
   <si>
     <t>人物ID_CharacterID</t>
   </si>
@@ -117,9 +117,6 @@
     <t>医者</t>
   </si>
   <si>
-    <t>Doctor</t>
-  </si>
-  <si>
     <t>中级医者</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>魔狼</t>
   </si>
   <si>
-    <t>Canis</t>
-  </si>
-  <si>
     <t>野狼</t>
   </si>
   <si>
@@ -603,24 +597,15 @@
     <t>黑鹰</t>
   </si>
   <si>
-    <t>Blackhawk</t>
-  </si>
-  <si>
     <t>格罗瓦兹商人</t>
   </si>
   <si>
     <t>格罗瓦兹</t>
   </si>
   <si>
-    <t>Gizeh</t>
-  </si>
-  <si>
     <t>野火</t>
   </si>
   <si>
-    <t>Wildfire</t>
-  </si>
-  <si>
     <t>匿名提可沁</t>
   </si>
   <si>
@@ -666,9 +651,6 @@
     <t>伊潘图</t>
   </si>
   <si>
-    <t>Ishtar</t>
-  </si>
-  <si>
     <t>英雄隆达</t>
   </si>
   <si>
@@ -687,258 +669,21 @@
     <t>拉拉队</t>
   </si>
   <si>
-    <t>Defensor General</t>
-  </si>
-  <si>
-    <t>Guardia</t>
-  </si>
-  <si>
-    <t>Herrero</t>
-  </si>
-  <si>
-    <t>Comerciante</t>
-  </si>
-  <si>
-    <t>Mensajero</t>
-  </si>
-  <si>
     <t>Comerciante Místico</t>
   </si>
   <si>
-    <t>Comerciante pasando</t>
-  </si>
-  <si>
-    <t>Comerciante de Intel</t>
-  </si>
-  <si>
-    <t>Trabajador</t>
-  </si>
-  <si>
-    <t>Herbolario</t>
-  </si>
-  <si>
-    <t>Forjador de espadas</t>
-  </si>
-  <si>
-    <t>Extraño Furudian</t>
-  </si>
-  <si>
-    <t>Guerrero Novato</t>
-  </si>
-  <si>
-    <t>Soldado Grunt</t>
-  </si>
-  <si>
-    <t>Comerciante Oasis</t>
-  </si>
-  <si>
-    <t>Jabalí</t>
-  </si>
-  <si>
-    <t>Lobo Salvaje</t>
-  </si>
-  <si>
-    <t>Conejo saltarín</t>
-  </si>
-  <si>
-    <t>Hada</t>
-  </si>
-  <si>
-    <t>Nasir Rey</t>
-  </si>
-  <si>
-    <t>Guerrero Bestia</t>
-  </si>
-  <si>
-    <t>Estatua antigua</t>
-  </si>
-  <si>
-    <t>Buey</t>
-  </si>
-  <si>
-    <t>Zorro</t>
-  </si>
-  <si>
-    <t>Gusano de arena 1</t>
-  </si>
-  <si>
-    <t>Escorpión 1</t>
-  </si>
-  <si>
-    <t>Serpiente 1</t>
-  </si>
-  <si>
-    <t>Águila 1</t>
-  </si>
-  <si>
     <t>Bandido</t>
   </si>
   <si>
-    <t>Guerrero Desconocido</t>
-  </si>
-  <si>
-    <t>Líder desconocido</t>
-  </si>
-  <si>
-    <t>Mercenario</t>
-  </si>
-  <si>
-    <t>Discípulo de la llama</t>
-  </si>
-  <si>
-    <t>Llama Doyen</t>
-  </si>
-  <si>
-    <t>Mago Ifrit</t>
-  </si>
-  <si>
-    <t>Enviado secreto</t>
-  </si>
-  <si>
-    <t>Guardia Real</t>
-  </si>
-  <si>
-    <t>¿?</t>
-  </si>
-  <si>
-    <t>Espiritumancer</t>
-  </si>
-  <si>
-    <t>Comerciante de madera</t>
-  </si>
-  <si>
-    <t>Comerciante de piedra de hierro</t>
-  </si>
-  <si>
-    <t>Comerciante de armas</t>
-  </si>
-  <si>
-    <t>Mercader de armaduras</t>
-  </si>
-  <si>
-    <t>Comerciante de empeños</t>
-  </si>
-  <si>
-    <t>Mercader de boticario</t>
-  </si>
-  <si>
-    <t>Comerciante de pergaminos</t>
-  </si>
-  <si>
-    <t>Comerciante de equipo</t>
-  </si>
-  <si>
-    <t>Comerciante de joyas</t>
-  </si>
-  <si>
-    <t>Botica Mística</t>
-  </si>
-  <si>
-    <t>Comerciante de baratijas</t>
-  </si>
-  <si>
     <t>Comerciante de Amuletos Místicos</t>
   </si>
   <si>
-    <t>Entrenamiento de Arcana de Fuego Ⅰ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Fuego Ⅱ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Fuego Ⅲ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Fuego Ⅳ</t>
-  </si>
-  <si>
-    <t>Entrenamiento del Arcano del Trueno Ⅰ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Luz Ⅱ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Alquimia Ⅲ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Hielo Ⅰ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana Oscura Ⅱ</t>
-  </si>
-  <si>
-    <t>Entrenamiento de Arcana de Hielo Ⅲ</t>
-  </si>
-  <si>
-    <t>Árbitro</t>
-  </si>
-  <si>
-    <t>Mensajero de Pergamino de Regreso</t>
-  </si>
-  <si>
     <t>Agricultor</t>
   </si>
   <si>
-    <t>Cazador</t>
-  </si>
-  <si>
-    <t>Minero</t>
-  </si>
-  <si>
-    <t>Criado del hotel</t>
-  </si>
-  <si>
-    <t>Guerrero caído</t>
-  </si>
-  <si>
-    <t>Sembrador</t>
-  </si>
-  <si>
-    <t>Ifrit regordete</t>
-  </si>
-  <si>
-    <t>Tuya</t>
-  </si>
-  <si>
-    <t>Canciones</t>
-  </si>
-  <si>
-    <t>Botica</t>
-  </si>
-  <si>
     <t>Florista</t>
   </si>
   <si>
-    <t>Anciano</t>
-  </si>
-  <si>
-    <t>Minero Jefe</t>
-  </si>
-  <si>
-    <t>Espíritu de Blackrock</t>
-  </si>
-  <si>
-    <t>Vendedor de vinos Blackrock</t>
-  </si>
-  <si>
-    <t>Mercader de armas de Blackrock</t>
-  </si>
-  <si>
-    <t>Soldado de la Legión de Ceniza de Blackrock</t>
-  </si>
-  <si>
-    <t>Gobernador de la Ciudad de Jamal</t>
-  </si>
-  <si>
-    <t>Jamal Gobernador Guardia</t>
-  </si>
-  <si>
-    <t>Chica misteriosa</t>
-  </si>
-  <si>
-    <t>Chica del cañón</t>
-  </si>
-  <si>
     <t>Líder A</t>
   </si>
   <si>
@@ -948,59 +693,318 @@
     <t>Líder C</t>
   </si>
   <si>
-    <t>Viejo Rey</t>
-  </si>
-  <si>
-    <t>Anger</t>
-  </si>
-  <si>
-    <t>Anfitrión del torneo</t>
-  </si>
-  <si>
-    <t>Reclutador de torneos</t>
-  </si>
-  <si>
-    <t>Escuadrón de animadoras</t>
-  </si>
-  <si>
-    <t>Comerciante del Mercado Negro</t>
-  </si>
-  <si>
     <t>Comerciante Principal</t>
   </si>
   <si>
-    <t>Comerciante del Mercado</t>
-  </si>
-  <si>
-    <t>Comerciante Viajero</t>
-  </si>
-  <si>
-    <t>Adivina del Futuro</t>
-  </si>
-  <si>
-    <t>Dueño de la Tienda</t>
-  </si>
-  <si>
-    <t>Buscador de Tesoros</t>
-  </si>
-  <si>
-    <t>Líder de la Mafia</t>
-  </si>
-  <si>
-    <t>Guardia de Cabeza</t>
-  </si>
-  <si>
-    <t>Guerrero Experimentado</t>
+    <t>Advogado Geral</t>
+  </si>
+  <si>
+    <t>Guarda Chefe</t>
+  </si>
+  <si>
+    <t>Líder da máfia</t>
+  </si>
+  <si>
+    <t>Guarda</t>
+  </si>
+  <si>
+    <t>Caçador de tesouros</t>
+  </si>
+  <si>
+    <t>Dono da loja</t>
+  </si>
+  <si>
+    <t>ferreiro</t>
+  </si>
+  <si>
+    <t>Homem de negocios</t>
+  </si>
+  <si>
+    <t>Correio de entrega</t>
+  </si>
+  <si>
+    <t>Comerciante do Mercado Negro</t>
+  </si>
+  <si>
+    <t>Cartomante</t>
+  </si>
+  <si>
+    <t>Comerciante Viajante</t>
+  </si>
+  <si>
+    <t>Comerciante de Mercado</t>
+  </si>
+  <si>
+    <t>Doutor</t>
+  </si>
+  <si>
+    <t>Passagem de comerciante</t>
+  </si>
+  <si>
+    <t>Comerciante Intel</t>
+  </si>
+  <si>
+    <t>Trabalhador</t>
+  </si>
+  <si>
+    <t>Herbalista</t>
+  </si>
+  <si>
+    <t>Estranho Furudiano</t>
+  </si>
+  <si>
+    <t>Guerreiro Novato</t>
+  </si>
+  <si>
+    <t>Guerreiro Experiente</t>
+  </si>
+  <si>
+    <t>Soldado Grunhido</t>
+  </si>
+  <si>
+    <t>Comerciante Oásis</t>
+  </si>
+  <si>
+    <t>Porco selvagem</t>
+  </si>
+  <si>
+    <t>Canino</t>
+  </si>
+  <si>
+    <t>Lobo selvagem</t>
+  </si>
+  <si>
+    <t>coelho saltando</t>
+  </si>
+  <si>
+    <t>Fada</t>
+  </si>
+  <si>
+    <t>Rei Nasir</t>
+  </si>
+  <si>
+    <t>Besta Guerreira</t>
+  </si>
+  <si>
+    <t>estátua antiga</t>
+  </si>
+  <si>
+    <t>Boi</t>
+  </si>
+  <si>
+    <t>Raposa</t>
+  </si>
+  <si>
+    <t>Verme da areia 1</t>
+  </si>
+  <si>
+    <t>Escorpião 1</t>
+  </si>
+  <si>
+    <t>Cobra 1</t>
+  </si>
+  <si>
+    <t>Águia 1</t>
+  </si>
+  <si>
+    <t>Guerreiro Desconhecido</t>
+  </si>
+  <si>
+    <t>Líder desconhecido</t>
+  </si>
+  <si>
+    <t>Mercenário</t>
+  </si>
+  <si>
+    <t>Discípulo da chama</t>
+  </si>
+  <si>
+    <t>Lhama Doyen</t>
+  </si>
+  <si>
+    <t>Assistente Ifrit</t>
+  </si>
+  <si>
+    <t>enviado secreto</t>
+  </si>
+  <si>
+    <t>guarda Real</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Espiritualista</t>
+  </si>
+  <si>
+    <t>Comerciante de madeira</t>
+  </si>
+  <si>
+    <t>Comerciante de Pedra Ferro</t>
+  </si>
+  <si>
+    <t>traficante de armas</t>
+  </si>
+  <si>
+    <t>Comerciante de Armaduras</t>
+  </si>
+  <si>
+    <t>Revendedor de penhores</t>
+  </si>
+  <si>
+    <t>Comerciante Boticário</t>
+  </si>
+  <si>
+    <t>Comerciante de rolagem</t>
+  </si>
+  <si>
+    <t>Comerciante de Equipamentos</t>
+  </si>
+  <si>
+    <t>Comerciante de joias</t>
+  </si>
+  <si>
+    <t>Boticário Místico</t>
+  </si>
+  <si>
+    <t>Revendedor de bugigangas</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Fogo Ⅰ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Fogo Ⅱ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Fogo Ⅲ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Fogo Ⅳ</t>
+  </si>
+  <si>
+    <t>Treinamento do Arcano do Trovão Ⅰ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano Leve Ⅱ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Alquimia Ⅲ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Gelo Ⅰ</t>
+  </si>
+  <si>
+    <t>Treinamento de Arcanos Negros Ⅱ</t>
+  </si>
+  <si>
+    <t>Treinamento Arcano de Gelo Ⅲ</t>
+  </si>
+  <si>
+    <t>Juiz</t>
+  </si>
+  <si>
+    <t>Mensageiro de rolagem de retorno</t>
+  </si>
+  <si>
+    <t>Caçador</t>
+  </si>
+  <si>
+    <t>Mineiro</t>
+  </si>
+  <si>
+    <t>Empregado de hotel</t>
+  </si>
+  <si>
+    <t>guerreiro caído</t>
+  </si>
+  <si>
+    <t>Semeador</t>
+  </si>
+  <si>
+    <t>ifrit gordo</t>
+  </si>
+  <si>
+    <t>Seu</t>
+  </si>
+  <si>
+    <t>músicas</t>
+  </si>
+  <si>
+    <t>Drogaria</t>
+  </si>
+  <si>
+    <t>Velhote</t>
+  </si>
+  <si>
+    <t>Mineiro Chefe</t>
+  </si>
+  <si>
+    <t>Espírito da Rocha Negra</t>
+  </si>
+  <si>
+    <t>Vendedor de vinho Blackrock</t>
+  </si>
+  <si>
+    <t>Comerciante de Armas Rocha Negra</t>
+  </si>
+  <si>
+    <t>Soldado da Legião Cinza Negra da Rocha Negra</t>
+  </si>
+  <si>
+    <t>Governador da cidade de Jamal</t>
+  </si>
+  <si>
+    <t>Jamal Governador Guardia</t>
+  </si>
+  <si>
+    <t>Garota misteriosa</t>
+  </si>
+  <si>
+    <t>garota do desfiladeiro</t>
+  </si>
+  <si>
+    <t>Falcão</t>
+  </si>
+  <si>
+    <t>Gizé</t>
+  </si>
+  <si>
+    <t>incêndios</t>
+  </si>
+  <si>
+    <t>Velho Rei</t>
+  </si>
+  <si>
+    <t>Istar</t>
+  </si>
+  <si>
+    <t>Raiva</t>
+  </si>
+  <si>
+    <t>Anfitrião do torneio</t>
+  </si>
+  <si>
+    <t>Recrutador de torneio</t>
+  </si>
+  <si>
+    <t>equipe de torcida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1042,29 +1046,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{38BB2749-43DC-468D-8B7D-D1059D5CE3A9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1080,7 +1087,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1378,11 +1385,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
@@ -1419,8 +1426,8 @@
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>218</v>
+      <c r="C2" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -1436,8 +1443,8 @@
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>318</v>
+      <c r="C3" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -1453,8 +1460,8 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>317</v>
+      <c r="C4" s="6" t="s">
+        <v>223</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -1470,8 +1477,8 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>219</v>
+      <c r="C5" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
@@ -1487,8 +1494,8 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>316</v>
+      <c r="C6" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -1504,8 +1511,8 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>315</v>
+      <c r="C7" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
@@ -1521,8 +1528,8 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>220</v>
+      <c r="C8" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
@@ -1538,8 +1545,8 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>221</v>
+      <c r="C9" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
@@ -1555,8 +1562,8 @@
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>222</v>
+      <c r="C10" s="6" t="s">
+        <v>229</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
@@ -1572,8 +1579,8 @@
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>222</v>
+      <c r="C11" s="6" t="s">
+        <v>229</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>7</v>
@@ -1589,8 +1596,8 @@
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>310</v>
+      <c r="C12" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -1606,8 +1613,8 @@
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>314</v>
+      <c r="C13" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
@@ -1623,8 +1630,8 @@
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
-        <v>313</v>
+      <c r="C14" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -1640,8 +1647,8 @@
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
-        <v>312</v>
+      <c r="C15" s="6" t="s">
+        <v>233</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1657,8 +1664,8 @@
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>311</v>
+      <c r="C16" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -1674,8 +1681,8 @@
       <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
+      <c r="C17" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -1686,13 +1693,13 @@
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
-        <v>28</v>
+      <c r="C18" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -1703,13 +1710,13 @@
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
-        <v>28</v>
+      <c r="C19" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -1720,13 +1727,13 @@
     </row>
     <row r="20" spans="1:6" ht="30">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>223</v>
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
@@ -1737,13 +1744,13 @@
     </row>
     <row r="21" spans="1:6" ht="30">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>224</v>
+        <v>31</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
@@ -1754,13 +1761,13 @@
     </row>
     <row r="22" spans="1:6" ht="30">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>225</v>
+        <v>32</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -1771,13 +1778,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>226</v>
+        <v>33</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>7</v>
@@ -1788,13 +1795,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>227</v>
+        <v>34</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>7</v>
@@ -1805,13 +1812,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>228</v>
+        <v>35</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -1822,13 +1829,13 @@
     </row>
     <row r="26" spans="1:6" ht="30">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>229</v>
+        <v>36</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>7</v>
@@ -1839,13 +1846,13 @@
     </row>
     <row r="27" spans="1:6" ht="30">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>230</v>
+        <v>37</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>7</v>
@@ -1856,13 +1863,13 @@
     </row>
     <row r="28" spans="1:6" ht="30">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>319</v>
+        <v>38</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>7</v>
@@ -1873,13 +1880,13 @@
     </row>
     <row r="29" spans="1:6" ht="30">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>231</v>
+        <v>39</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>7</v>
@@ -1890,13 +1897,13 @@
     </row>
     <row r="30" spans="1:6" ht="30">
       <c r="A30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" t="s">
-        <v>232</v>
+      <c r="C30" s="6" t="s">
+        <v>243</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>7</v>
@@ -1912,8 +1919,8 @@
       <c r="B31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C31" t="s">
-        <v>313</v>
+      <c r="C31" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>7</v>
@@ -1924,13 +1931,13 @@
     </row>
     <row r="32" spans="1:6" ht="30">
       <c r="A32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C32" t="s">
-        <v>313</v>
+      <c r="C32" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
@@ -1941,13 +1948,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>233</v>
+        <v>43</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
@@ -1958,13 +1965,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>7</v>
@@ -1975,13 +1982,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" t="s">
-        <v>234</v>
+        <v>45</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>7</v>
@@ -1992,13 +1999,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" t="s">
-        <v>235</v>
+        <v>47</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>7</v>
@@ -2009,13 +2016,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>236</v>
+        <v>48</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>248</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>7</v>
@@ -2026,13 +2033,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" t="s">
-        <v>237</v>
+        <v>49</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>249</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>7</v>
@@ -2043,13 +2050,13 @@
     </row>
     <row r="39" spans="1:6" ht="30">
       <c r="A39" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" t="s">
-        <v>238</v>
+        <v>50</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>7</v>
@@ -2060,13 +2067,13 @@
     </row>
     <row r="40" spans="1:6" ht="30">
       <c r="A40" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" t="s">
-        <v>239</v>
+        <v>51</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>7</v>
@@ -2077,13 +2084,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" t="s">
-        <v>240</v>
+        <v>53</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>252</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>7</v>
@@ -2094,13 +2101,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" t="s">
-        <v>241</v>
+        <v>55</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>7</v>
@@ -2111,13 +2118,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" t="s">
-        <v>242</v>
+        <v>56</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>7</v>
@@ -2128,13 +2135,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" t="s">
-        <v>243</v>
+        <v>57</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -2145,13 +2152,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" t="s">
-        <v>244</v>
+        <v>58</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>7</v>
@@ -2162,13 +2169,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>245</v>
+        <v>59</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>257</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>7</v>
@@ -2179,13 +2186,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" t="s">
-        <v>246</v>
+        <v>60</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>7</v>
@@ -2196,13 +2203,13 @@
     </row>
     <row r="48" spans="1:6" ht="30">
       <c r="A48" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" t="s">
-        <v>247</v>
+        <v>62</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>7</v>
@@ -2213,13 +2220,13 @@
     </row>
     <row r="49" spans="1:6" ht="30">
       <c r="A49" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" t="s">
-        <v>247</v>
+        <v>62</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>7</v>
@@ -2230,13 +2237,13 @@
     </row>
     <row r="50" spans="1:6" ht="45">
       <c r="A50" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" t="s">
-        <v>248</v>
+        <v>65</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>7</v>
@@ -2247,13 +2254,13 @@
     </row>
     <row r="51" spans="1:6" ht="30">
       <c r="A51" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s">
-        <v>249</v>
+        <v>67</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>7</v>
@@ -2264,13 +2271,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" t="s">
-        <v>219</v>
+        <v>68</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>7</v>
@@ -2281,13 +2288,13 @@
     </row>
     <row r="53" spans="1:6" ht="30">
       <c r="A53" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" t="s">
-        <v>250</v>
+        <v>70</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>7</v>
@@ -2298,13 +2305,13 @@
     </row>
     <row r="54" spans="1:6" ht="45">
       <c r="A54" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C54" t="s">
-        <v>251</v>
+        <v>72</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>262</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>7</v>
@@ -2315,13 +2322,13 @@
     </row>
     <row r="55" spans="1:6" ht="30">
       <c r="A55" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" t="s">
-        <v>252</v>
+        <v>73</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>7</v>
@@ -2332,13 +2339,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" t="s">
-        <v>253</v>
+        <v>74</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>7</v>
@@ -2349,13 +2356,13 @@
     </row>
     <row r="57" spans="1:6" ht="30">
       <c r="A57" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" t="s">
-        <v>254</v>
+        <v>75</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>7</v>
@@ -2366,13 +2373,13 @@
     </row>
     <row r="58" spans="1:6" ht="30">
       <c r="A58" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" t="s">
-        <v>255</v>
+        <v>77</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>7</v>
@@ -2383,13 +2390,13 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" t="s">
-        <v>255</v>
+        <v>77</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>7</v>
@@ -2400,13 +2407,13 @@
     </row>
     <row r="60" spans="1:6" ht="30">
       <c r="A60" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" t="s">
-        <v>256</v>
+        <v>80</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>7</v>
@@ -2417,13 +2424,13 @@
     </row>
     <row r="61" spans="1:6" ht="30">
       <c r="A61" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" t="s">
-        <v>257</v>
+        <v>81</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>7</v>
@@ -2434,13 +2441,13 @@
     </row>
     <row r="62" spans="1:6" ht="30">
       <c r="A62" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C62" t="s">
-        <v>258</v>
+        <v>82</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>7</v>
@@ -2451,13 +2458,13 @@
     </row>
     <row r="63" spans="1:6" ht="30">
       <c r="A63" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" t="s">
-        <v>221</v>
+        <v>84</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>7</v>
@@ -2468,13 +2475,13 @@
     </row>
     <row r="64" spans="1:6" ht="45">
       <c r="A64" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" t="s">
-        <v>259</v>
+        <v>86</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>7</v>
@@ -2485,13 +2492,13 @@
     </row>
     <row r="65" spans="1:6" ht="45">
       <c r="A65" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" t="s">
-        <v>260</v>
+        <v>88</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>7</v>
@@ -2502,13 +2509,13 @@
     </row>
     <row r="66" spans="1:6" ht="45">
       <c r="A66" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" t="s">
-        <v>261</v>
+        <v>90</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>7</v>
@@ -2519,13 +2526,13 @@
     </row>
     <row r="67" spans="1:6" ht="45">
       <c r="A67" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" t="s">
-        <v>223</v>
+        <v>30</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>7</v>
@@ -2536,13 +2543,13 @@
     </row>
     <row r="68" spans="1:6" ht="45">
       <c r="A68" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" t="s">
-        <v>262</v>
+        <v>93</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
@@ -2553,13 +2560,13 @@
     </row>
     <row r="69" spans="1:6" ht="45">
       <c r="A69" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" t="s">
-        <v>263</v>
+        <v>95</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>7</v>
@@ -2570,13 +2577,13 @@
     </row>
     <row r="70" spans="1:6" ht="45">
       <c r="A70" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" t="s">
-        <v>264</v>
+        <v>97</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>7</v>
@@ -2587,13 +2594,13 @@
     </row>
     <row r="71" spans="1:6" ht="45">
       <c r="A71" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" t="s">
-        <v>223</v>
+        <v>30</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>7</v>
@@ -2604,13 +2611,13 @@
     </row>
     <row r="72" spans="1:6" ht="45">
       <c r="A72" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" t="s">
-        <v>264</v>
+        <v>97</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>7</v>
@@ -2621,13 +2628,13 @@
     </row>
     <row r="73" spans="1:6" ht="45">
       <c r="A73" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C73" t="s">
-        <v>265</v>
+        <v>101</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>7</v>
@@ -2638,13 +2645,13 @@
     </row>
     <row r="74" spans="1:6" ht="45">
       <c r="A74" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C74" t="s">
-        <v>266</v>
+        <v>103</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>7</v>
@@ -2655,13 +2662,13 @@
     </row>
     <row r="75" spans="1:6" ht="45">
       <c r="A75" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" t="s">
-        <v>267</v>
+        <v>105</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>278</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>7</v>
@@ -2672,13 +2679,13 @@
     </row>
     <row r="76" spans="1:6" ht="45">
       <c r="A76" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C76" t="s">
-        <v>268</v>
+        <v>107</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>7</v>
@@ -2689,13 +2696,13 @@
     </row>
     <row r="77" spans="1:6" ht="30">
       <c r="A77" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" t="s">
-        <v>269</v>
+        <v>109</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>7</v>
@@ -2706,13 +2713,13 @@
     </row>
     <row r="78" spans="1:6" ht="45">
       <c r="A78" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C78" t="s">
-        <v>270</v>
+        <v>111</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>280</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>7</v>
@@ -2723,13 +2730,13 @@
     </row>
     <row r="79" spans="1:6" ht="45">
       <c r="A79" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C79" t="s">
-        <v>271</v>
+        <v>113</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>281</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>7</v>
@@ -2740,13 +2747,13 @@
     </row>
     <row r="80" spans="1:6" ht="45">
       <c r="A80" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C80" t="s">
-        <v>272</v>
+        <v>115</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>7</v>
@@ -2757,13 +2764,13 @@
     </row>
     <row r="81" spans="1:6" ht="30">
       <c r="A81" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" t="s">
-        <v>273</v>
+        <v>117</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>7</v>
@@ -2774,13 +2781,13 @@
     </row>
     <row r="82" spans="1:6" ht="30">
       <c r="A82" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C82" t="s">
-        <v>274</v>
+        <v>119</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>7</v>
@@ -2791,13 +2798,13 @@
     </row>
     <row r="83" spans="1:6" ht="30">
       <c r="A83" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83" t="s">
-        <v>275</v>
+        <v>121</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>7</v>
@@ -2808,13 +2815,13 @@
     </row>
     <row r="84" spans="1:6" ht="45">
       <c r="A84" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C84" t="s">
-        <v>276</v>
+        <v>123</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>7</v>
@@ -2825,13 +2832,13 @@
     </row>
     <row r="85" spans="1:6" ht="30">
       <c r="A85" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C85" t="s">
-        <v>277</v>
+        <v>125</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>7</v>
@@ -2842,13 +2849,13 @@
     </row>
     <row r="86" spans="1:6" ht="30">
       <c r="A86" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C86" t="s">
-        <v>278</v>
+        <v>127</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>7</v>
@@ -2859,13 +2866,13 @@
     </row>
     <row r="87" spans="1:6" ht="30">
       <c r="A87" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C87" t="s">
-        <v>279</v>
+        <v>128</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>7</v>
@@ -2876,13 +2883,13 @@
     </row>
     <row r="88" spans="1:6" ht="30">
       <c r="A88" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C88" t="s">
-        <v>280</v>
+        <v>130</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>7</v>
@@ -2893,13 +2900,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C89" t="s">
-        <v>281</v>
+        <v>132</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>7</v>
@@ -2910,13 +2917,13 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C90" t="s">
-        <v>281</v>
+        <v>132</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>7</v>
@@ -2927,13 +2934,13 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C91" t="s">
-        <v>281</v>
+        <v>132</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>7</v>
@@ -2944,13 +2951,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C92" t="s">
-        <v>281</v>
+        <v>132</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>7</v>
@@ -2961,13 +2968,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C93" t="s">
-        <v>281</v>
+        <v>132</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>7</v>
@@ -2978,13 +2985,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C94" t="s">
-        <v>282</v>
+        <v>137</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>7</v>
@@ -2995,13 +3002,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C95" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>7</v>
@@ -3012,13 +3019,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C96" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>7</v>
@@ -3029,13 +3036,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C97" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>7</v>
@@ -3046,13 +3053,13 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C98" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>7</v>
@@ -3063,13 +3070,13 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C99" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>7</v>
@@ -3080,13 +3087,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C100" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>7</v>
@@ -3097,13 +3104,13 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C101" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>7</v>
@@ -3114,13 +3121,13 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C102" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>7</v>
@@ -3131,13 +3138,13 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C103" t="s">
-        <v>283</v>
+        <v>138</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>7</v>
@@ -3148,13 +3155,13 @@
     </row>
     <row r="104" spans="1:6" ht="30">
       <c r="A104" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C104" t="s">
-        <v>284</v>
+        <v>147</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>293</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>7</v>
@@ -3165,13 +3172,13 @@
     </row>
     <row r="105" spans="1:6" ht="30">
       <c r="A105" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C105" t="s">
-        <v>285</v>
+        <v>148</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>7</v>
@@ -3182,13 +3189,13 @@
     </row>
     <row r="106" spans="1:6" ht="30">
       <c r="A106" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C106" t="s">
-        <v>286</v>
+        <v>150</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>295</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>7</v>
@@ -3199,13 +3206,13 @@
     </row>
     <row r="107" spans="1:6" ht="30">
       <c r="A107" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C107" t="s">
-        <v>287</v>
+        <v>151</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>7</v>
@@ -3216,13 +3223,13 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C108" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>7</v>
@@ -3233,13 +3240,13 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C109" t="s">
-        <v>157</v>
+        <v>154</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>7</v>
@@ -3250,13 +3257,13 @@
     </row>
     <row r="110" spans="1:6" ht="30">
       <c r="A110" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C110" t="s">
-        <v>288</v>
+        <v>157</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>7</v>
@@ -3267,13 +3274,13 @@
     </row>
     <row r="111" spans="1:6" ht="45">
       <c r="A111" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C111" t="s">
-        <v>289</v>
+        <v>159</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>7</v>
@@ -3284,13 +3291,13 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C112" t="s">
-        <v>290</v>
+        <v>160</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>7</v>
@@ -3301,13 +3308,13 @@
     </row>
     <row r="113" spans="1:6" ht="30">
       <c r="A113" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C113" t="s">
-        <v>247</v>
+        <v>62</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>7</v>
@@ -3318,13 +3325,13 @@
     </row>
     <row r="114" spans="1:6" ht="30">
       <c r="A114" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C114" t="s">
-        <v>291</v>
+        <v>163</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>216</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>7</v>
@@ -3335,13 +3342,13 @@
     </row>
     <row r="115" spans="1:6" ht="30">
       <c r="A115" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C115" t="s">
-        <v>292</v>
+        <v>165</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>7</v>
@@ -3352,13 +3359,13 @@
     </row>
     <row r="116" spans="1:6" ht="30">
       <c r="A116" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C116" t="s">
-        <v>220</v>
+      <c r="C116" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>7</v>
@@ -3369,13 +3376,13 @@
     </row>
     <row r="117" spans="1:6" ht="30">
       <c r="A117" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C117" t="s">
-        <v>256</v>
+        <v>80</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>7</v>
@@ -3386,13 +3393,13 @@
     </row>
     <row r="118" spans="1:6" ht="30">
       <c r="A118" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C118" t="s">
-        <v>228</v>
+        <v>35</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>7</v>
@@ -3403,13 +3410,13 @@
     </row>
     <row r="119" spans="1:6" ht="30">
       <c r="A119" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C119" t="s">
-        <v>293</v>
+        <v>170</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>301</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>7</v>
@@ -3420,13 +3427,13 @@
     </row>
     <row r="120" spans="1:6" ht="30">
       <c r="A120" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C120" t="s">
-        <v>221</v>
+        <v>84</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>7</v>
@@ -3437,13 +3444,13 @@
     </row>
     <row r="121" spans="1:6" ht="30">
       <c r="A121" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C121" t="s">
-        <v>260</v>
+        <v>88</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>7</v>
@@ -3454,13 +3461,13 @@
     </row>
     <row r="122" spans="1:6" ht="30">
       <c r="A122" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C122" t="s">
-        <v>294</v>
+        <v>173</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>302</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>7</v>
@@ -3471,13 +3478,13 @@
     </row>
     <row r="123" spans="1:6" ht="30">
       <c r="A123" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C123" t="s">
-        <v>295</v>
+        <v>174</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>303</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>7</v>
@@ -3488,13 +3495,13 @@
     </row>
     <row r="124" spans="1:6" ht="30">
       <c r="A124" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" t="s">
-        <v>296</v>
+        <v>175</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>304</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>7</v>
@@ -3505,13 +3512,13 @@
     </row>
     <row r="125" spans="1:6" ht="45">
       <c r="A125" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C125" t="s">
-        <v>297</v>
+        <v>176</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>7</v>
@@ -3522,13 +3529,13 @@
     </row>
     <row r="126" spans="1:6" ht="30">
       <c r="A126" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C126" t="s">
-        <v>298</v>
+        <v>177</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>7</v>
@@ -3539,13 +3546,13 @@
     </row>
     <row r="127" spans="1:6" ht="45">
       <c r="A127" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C127" t="s">
-        <v>299</v>
+        <v>178</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>307</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>7</v>
@@ -3556,13 +3563,13 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C128" t="s">
-        <v>182</v>
+        <v>179</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>7</v>
@@ -3573,13 +3580,13 @@
     </row>
     <row r="129" spans="1:6" ht="30">
       <c r="A129" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C129" t="s">
-        <v>300</v>
+        <v>182</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>308</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>7</v>
@@ -3590,13 +3597,13 @@
     </row>
     <row r="130" spans="1:6" ht="30">
       <c r="A130" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C130" t="s">
-        <v>301</v>
+        <v>183</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>309</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>7</v>
@@ -3607,13 +3614,13 @@
     </row>
     <row r="131" spans="1:6" ht="30">
       <c r="A131" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C131" t="s">
-        <v>255</v>
+        <v>77</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>7</v>
@@ -3624,13 +3631,13 @@
     </row>
     <row r="132" spans="1:6" ht="30">
       <c r="A132" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C132" t="s">
-        <v>255</v>
+        <v>77</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>7</v>
@@ -3641,13 +3648,13 @@
     </row>
     <row r="133" spans="1:6" ht="30">
       <c r="A133" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C133" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>310</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>7</v>
@@ -3658,13 +3665,13 @@
     </row>
     <row r="134" spans="1:6" ht="30">
       <c r="A134" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C134" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>311</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>7</v>
@@ -3675,13 +3682,13 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C135" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>7</v>
@@ -3692,13 +3699,13 @@
     </row>
     <row r="136" spans="1:6" ht="30">
       <c r="A136" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C136" t="s">
-        <v>300</v>
+        <v>192</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>308</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>7</v>
@@ -3709,13 +3716,13 @@
     </row>
     <row r="137" spans="1:6" ht="45">
       <c r="A137" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C137" t="s">
-        <v>302</v>
+        <v>194</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>217</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>7</v>
@@ -3726,13 +3733,13 @@
     </row>
     <row r="138" spans="1:6" ht="45">
       <c r="A138" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C138" t="s">
-        <v>303</v>
+        <v>196</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>7</v>
@@ -3743,13 +3750,13 @@
     </row>
     <row r="139" spans="1:6" ht="45">
       <c r="A139" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C139" t="s">
-        <v>304</v>
+        <v>198</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>7</v>
@@ -3760,13 +3767,13 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C140" t="s">
-        <v>205</v>
+        <v>199</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>200</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>7</v>
@@ -3777,13 +3784,13 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C141" t="s">
-        <v>305</v>
+        <v>201</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>7</v>
@@ -3794,13 +3801,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C142" t="s">
-        <v>208</v>
+        <v>202</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="D142" s="4" t="s">
         <v>7</v>
@@ -3811,13 +3818,13 @@
     </row>
     <row r="143" spans="1:6" ht="30">
       <c r="A143" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C143" t="s">
-        <v>211</v>
+        <v>205</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="D143" s="4" t="s">
         <v>7</v>
@@ -3828,13 +3835,13 @@
     </row>
     <row r="144" spans="1:6" ht="30">
       <c r="A144" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C144" t="s">
-        <v>306</v>
+        <v>207</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>315</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>7</v>
@@ -3845,13 +3852,13 @@
     </row>
     <row r="145" spans="1:6" ht="45">
       <c r="A145" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C145" t="s">
-        <v>307</v>
+        <v>208</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>7</v>
@@ -3862,13 +3869,13 @@
     </row>
     <row r="146" spans="1:6" ht="30">
       <c r="A146" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C146" t="s">
-        <v>308</v>
+        <v>209</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>7</v>
@@ -3879,13 +3886,13 @@
     </row>
     <row r="147" spans="1:6" ht="30">
       <c r="A147" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C147" t="s">
-        <v>309</v>
+        <v>211</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>7</v>

</xml_diff>